<commit_message>
updated supp table 3
</commit_message>
<xml_diff>
--- a/tactical_analyses/manuscript/Supplementary_Tables.xlsx
+++ b/tactical_analyses/manuscript/Supplementary_Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="28700" windowHeight="17540" tabRatio="710"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28700" windowHeight="17540" tabRatio="710" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary Table 1" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="supp_table_2a" localSheetId="1">'Supplementary Table 2'!$A$6:$L$13</definedName>
     <definedName name="supp_table_2b" localSheetId="1">'Supplementary Table 2'!$A$15:$L$47</definedName>
     <definedName name="supp_table_2c" localSheetId="1">'Supplementary Table 2'!$A$49:$L$149</definedName>
+    <definedName name="supp_table_3" localSheetId="2">'Supplementary Table 3'!$A$14:$D$17</definedName>
     <definedName name="supptab1" localSheetId="0">'Supplementary Table 1'!$B$3:$O$4</definedName>
     <definedName name="SuppTable_shared_tier1" localSheetId="1">'Supplementary Table 2'!$A$3:$L$13</definedName>
     <definedName name="table_eqtls_prettyNum" localSheetId="4">'Supplementary Table 5'!$A$3:$N$59</definedName>
@@ -103,7 +104,7 @@
     </textPr>
   </connection>
   <connection id="6" name="supp_table_2a.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2a.csv" comma="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2a.csv" comma="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -121,7 +122,7 @@
     </textPr>
   </connection>
   <connection id="7" name="supp_table_2b.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2b.csv" tab="0" comma="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2b.csv" tab="0" comma="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -139,7 +140,7 @@
     </textPr>
   </connection>
   <connection id="8" name="supp_table_2c.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2c.csv" tab="0" comma="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_2c.csv" tab="0" comma="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -156,14 +157,24 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="supptab1.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="supp_table_3.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="Macintosh HD:Users:jtorres:Google Drive:Science:Projects:t2d_classification:tactical_analyses:manuscript:table_files:supp_table_3.txt">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" name="supptab1.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:TEMPO:supptab1.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="SuppTable_shared_tier1.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="SuppTable_shared_tier1.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:TEMPO:SuppTable_shared_tier1.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -181,7 +192,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="SuppTable_shared_tier2.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="12" name="SuppTable_shared_tier2.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:TEMPO:SuppTable_shared_tier2.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -199,7 +210,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="SuppTable_shared_tier3.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="SuppTable_shared_tier3.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:TEMPO:SuppTable_shared_tier3.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -217,7 +228,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="table_eqtls_prettyNum.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="14" name="table_eqtls_prettyNum.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:Desktop:Temp:table_eqtls_prettyNum.txt">
       <textFields count="14">
         <textField/>
@@ -237,7 +248,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="table_islet_genes_prettyNum.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="15" name="table_islet_genes_prettyNum.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:jtorres:Desktop:Temp:table_islet_genes_prettyNum.txt">
       <textFields count="18">
         <textField/>
@@ -6610,7 +6621,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6651,6 +6662,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6672,6 +6686,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6681,14 +6701,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -6736,39 +6753,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supptab1" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_1" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="table_eqtls_prettyNum" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_1" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supptab1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SuppTable_shared_tier1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_2a" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_2a" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SuppTable_shared_tier1" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_2c" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_2b" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_2c" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="supp_table_3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="brain-enrich" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="coloc_380_clpp01_allpairs_expanded_ppa50" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="table_eqtls_prettyNum" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7095,7 +7116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
@@ -7120,77 +7141,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>1542</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>1541</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>889</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>1540</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>891</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>892</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>893</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>1814</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="25" t="s">
         <v>1810</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25" t="s">
         <v>1802</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="13" t="s">
         <v>1808</v>
       </c>
@@ -25249,37 +25270,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1834</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="20" t="s">
         <v>1830</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>888</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -25288,26 +25309,26 @@
       <c r="G3" s="20" t="s">
         <v>1828</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="25" t="s">
         <v>1832</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:12" ht="45">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="22" t="s">
         <v>1831</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="32" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="22" t="s">
         <v>1827</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="22" t="s">
         <v>1829</v>
       </c>
       <c r="H4" s="20" t="s">
@@ -30772,12 +30793,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H3:L3"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="H3:L3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -30790,18 +30811,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
@@ -30812,164 +30833,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>1841</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" ht="40" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>1797</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>1815</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25" t="s">
         <v>1798</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="13" t="s">
         <v>1817</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1816</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="35" t="s">
         <v>1799</v>
       </c>
       <c r="B8" s="18">
-        <v>6.0862423605442199E-3</v>
+        <v>6.7412817422222203E-3</v>
       </c>
       <c r="C8" s="18">
-        <v>0.12747884101627899</v>
+        <v>0.16352356665538501</v>
       </c>
       <c r="D8" s="10">
-        <v>2.3657410925768002E-3</v>
+        <v>7.8530099969105396E-3</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="35" t="s">
         <v>1800</v>
       </c>
       <c r="B9" s="18">
-        <v>9.1010660020408203E-3</v>
+        <v>2.2750699726349199E-2</v>
       </c>
       <c r="C9" s="18">
-        <v>0.26551377546162802</v>
+        <v>0.28220657970000002</v>
       </c>
       <c r="D9" s="11">
-        <v>1.00209445616966E-14</v>
+        <v>9.2141167408760902E-11</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="35" t="s">
         <v>1840</v>
       </c>
       <c r="B10" s="18">
-        <v>0.15601847003571401</v>
+        <v>0.14708938495841301</v>
       </c>
       <c r="C10" s="18">
-        <v>2.9572887081395299E-2</v>
+        <v>3.1992957193846198E-2</v>
       </c>
       <c r="D10" s="11">
-        <v>2.00715839097636E-5</v>
+        <v>7.53255095625393E-5</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="36" t="s">
         <v>1801</v>
       </c>
       <c r="B11" s="19">
-        <v>4.6549401129932E-2</v>
+        <v>4.34971738609524E-2</v>
       </c>
       <c r="C11" s="19">
-        <v>5.3448399872093001E-3</v>
+        <v>6.8241600753846197E-3</v>
       </c>
       <c r="D11" s="12">
-        <v>3.7416961002024199E-4</v>
-      </c>
+        <v>5.3978081130849698E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -31009,78 +31036,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>1825</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>1818</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>1819</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>891</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>892</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="26" t="s">
         <v>1820</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>1548</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="25" t="s">
         <v>1821</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="26" t="s">
         <v>1824</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="25" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="13" t="s">
         <v>1822</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>1823</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
@@ -43229,82 +43256,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>1835</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>888</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>889</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>890</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>891</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>892</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>1807</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="25" t="s">
         <v>893</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="25" t="s">
         <v>1809</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="13" t="s">
         <v>1836</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="25" t="s">
         <v>1838</v>
       </c>
-      <c r="O3" s="24"/>
+      <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="13" t="s">
         <v>1549</v>
       </c>
@@ -43320,7 +43347,7 @@
       <c r="L4" s="13" t="s">
         <v>1837</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="25"/>
       <c r="N4" s="13" t="s">
         <v>1839</v>
       </c>

</xml_diff>